<commit_message>
updated export alert tool
</commit_message>
<xml_diff>
--- a/tooling/export-alerts/alerts-template.xlsx
+++ b/tooling/export-alerts/alerts-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jabar\repos\azure-monitor-baseline-alerts\tooling\export-alerts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FD50A9D-FDF8-4677-87AA-4A1F5FAFDD3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EC45B96-E56E-481B-8458-48A49C7CB7A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7065" yWindow="1845" windowWidth="40725" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="2505" windowWidth="31890" windowHeight="19095" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metric Alerts" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="33">
   <si>
     <t>Resource Category</t>
   </si>
@@ -66,15 +66,15 @@
     <t>dimensions</t>
   </si>
   <si>
+    <t>alertSensitivity</t>
+  </si>
+  <si>
+    <t>failingPeriods</t>
+  </si>
+  <si>
     <t>references</t>
   </si>
   <si>
-    <t>alertSensitivity</t>
-  </si>
-  <si>
-    <t>failingPeriods</t>
-  </si>
-  <si>
     <t>metricMeasureColumn</t>
   </si>
   <si>
@@ -100,16 +100,43 @@
   </si>
   <si>
     <t>incidentType</t>
+  </si>
+  <si>
+    <t>visible</t>
+  </si>
+  <si>
+    <t>verified</t>
+  </si>
+  <si>
+    <t>tags</t>
+  </si>
+  <si>
+    <t>autoMitigate</t>
+  </si>
+  <si>
+    <t>autoResolve</t>
+  </si>
+  <si>
+    <t>autoResolveTime</t>
+  </si>
+  <si>
+    <t>z</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -160,13 +187,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="MetricAlerts" displayName="MetricAlerts" ref="A1:Q2" insertRow="1">
-  <autoFilter ref="A1:Q2" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="MetricAlerts" displayName="MetricAlerts" ref="A1:W2" insertRow="1">
+  <autoFilter ref="A1:W2" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="23">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Resource Category"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Resource Type"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Name"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Description"/>
+    <tableColumn id="19" xr3:uid="{476C6A71-89C4-4B21-B940-AE5B1CA84A2E}" name="visible"/>
+    <tableColumn id="15" xr3:uid="{2032A8E3-67CC-4BD6-B6CD-DAF646258DA2}" name="verified"/>
+    <tableColumn id="20" xr3:uid="{519C648D-F10B-4D7E-8B3A-8642212CB70A}" name="tags"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="metricName"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="metricNamespace"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="severity" dataDxfId="0"/>
@@ -179,20 +209,26 @@
     <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="dimensions"/>
     <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="alertSensitivity"/>
     <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="failingPeriods"/>
-    <tableColumn id="18" xr3:uid="{F3D398AC-A4AE-426C-9DE3-E28A7C831B3C}" name="references"/>
+    <tableColumn id="26" xr3:uid="{19C1C737-9F78-4200-8884-19A2B9C27770}" name="metricMeasureColumn"/>
+    <tableColumn id="27" xr3:uid="{C427348A-334B-4484-A1AA-891079A83CE9}" name="resouceIdColumn"/>
+    <tableColumn id="21" xr3:uid="{253BF780-4AB2-4CCF-9A8A-433F07FCB9B8}" name="autoMitigate"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="references"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="LogAlerts" displayName="LogAlerts" ref="A1:P2" insertRow="1">
-  <autoFilter ref="A1:P2" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <tableColumns count="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="LogAlerts" displayName="LogAlerts" ref="A1:V2" insertRow="1">
+  <autoFilter ref="A1:V2" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <tableColumns count="22">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Resource Category"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Resource Type"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Name"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Description"/>
+    <tableColumn id="21" xr3:uid="{F6B2E57F-58AF-4683-8EB1-A71B6B699766}" name="visible"/>
+    <tableColumn id="22" xr3:uid="{693129E0-D1DE-4ABF-8182-8B1C5CD099D1}" name="verified"/>
+    <tableColumn id="19" xr3:uid="{06A9E8ED-D969-40B5-8CF3-1FAE85BDDE11}" name="tags"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="severity"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="operator"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="timeAggregation"/>
@@ -204,6 +240,9 @@
     <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="dimensions"/>
     <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="failingPeriods"/>
     <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="query"/>
+    <tableColumn id="20" xr3:uid="{71E6D465-541C-40CF-BD9E-FE5B9B13A62E}" name="autoMitigate"/>
+    <tableColumn id="18" xr3:uid="{B6A334FF-FA59-4E60-8F2E-DED2EA6E50D9}" name="autoResolve"/>
+    <tableColumn id="17" xr3:uid="{BEC0AEB0-D731-4AC7-9015-A2C71A5ACDE7}" name="autoResolveTime"/>
     <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="references"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -211,20 +250,23 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="ActivityAlerts" displayName="ActivityAlerts" ref="A1:K2" insertRow="1">
-  <autoFilter ref="A1:K2" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
-  <tableColumns count="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="ActivityAlerts" displayName="ActivityAlerts" ref="A1:N2" insertRow="1">
+  <autoFilter ref="A1:N2" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Resource Category"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Resource Type"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Name"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Description"/>
+    <tableColumn id="13" xr3:uid="{9E87A1BA-04F4-4F90-9BE0-FE7578C74C2C}" name="visible"/>
+    <tableColumn id="12" xr3:uid="{E07D1F47-736A-4BEC-B910-FB0FAB0A427A}" name="verified"/>
+    <tableColumn id="14" xr3:uid="{FB1A8AE3-7645-4024-B90A-FF33DEC8116B}" name="tags"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="category"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="operationName"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="status"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="causes"/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="currentHealthStatus"/>
     <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="incidentType"/>
-    <tableColumn id="8" xr3:uid="{55D36F35-4ED6-4928-A75E-21D3F11FB426}" name="references"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="references"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -515,34 +557,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:W187"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="T1" sqref="T1:T1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="69.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="47.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="63.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="60.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="115.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" customWidth="1"/>
+    <col min="3" max="3" width="36.85546875" customWidth="1"/>
+    <col min="4" max="4" width="61.85546875" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="23.42578125" customWidth="1"/>
+    <col min="10" max="10" width="21.28515625" customWidth="1"/>
+    <col min="11" max="11" width="21.42578125" customWidth="1"/>
+    <col min="12" max="12" width="25.5703125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.85546875" customWidth="1"/>
+    <col min="18" max="18" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="23.5703125" customWidth="1"/>
+    <col min="20" max="20" width="23.85546875" customWidth="1"/>
+    <col min="21" max="21" width="21.28515625" customWidth="1"/>
+    <col min="22" max="22" width="18" customWidth="1"/>
+    <col min="23" max="23" width="40.42578125" customWidth="1"/>
+    <col min="24" max="24" width="60.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="60.28515625" customWidth="1"/>
+    <col min="26" max="26" width="115.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -556,62 +606,590 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
+        <v>14</v>
+      </c>
+      <c r="S1" t="s">
         <v>15</v>
       </c>
-      <c r="P1" t="s">
+      <c r="T1" t="s">
+        <v>17</v>
+      </c>
+      <c r="U1" t="s">
+        <v>18</v>
+      </c>
+      <c r="V1" t="s">
+        <v>29</v>
+      </c>
+      <c r="W1" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="G2"/>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="L2"/>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="L3"/>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="L4"/>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="L5"/>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="L6"/>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="L7"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="L8"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="L9"/>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="L10"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="L11"/>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="L12"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="L13"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="L14"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="L15"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="L16"/>
+    </row>
+    <row r="17" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L17"/>
+    </row>
+    <row r="18" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L18"/>
+    </row>
+    <row r="19" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L19"/>
+    </row>
+    <row r="20" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L20"/>
+    </row>
+    <row r="21" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L21"/>
+    </row>
+    <row r="22" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L22"/>
+    </row>
+    <row r="23" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L23"/>
+    </row>
+    <row r="24" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L24"/>
+    </row>
+    <row r="25" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L25"/>
+    </row>
+    <row r="26" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L26"/>
+    </row>
+    <row r="27" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L27"/>
+    </row>
+    <row r="28" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L28"/>
+    </row>
+    <row r="29" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L29"/>
+    </row>
+    <row r="30" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L30"/>
+    </row>
+    <row r="31" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L31"/>
+    </row>
+    <row r="32" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L32"/>
+    </row>
+    <row r="33" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L33"/>
+    </row>
+    <row r="34" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L34"/>
+    </row>
+    <row r="35" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L35"/>
+    </row>
+    <row r="36" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L36"/>
+    </row>
+    <row r="37" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L37"/>
+    </row>
+    <row r="38" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L38"/>
+    </row>
+    <row r="39" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L39"/>
+    </row>
+    <row r="40" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L40"/>
+    </row>
+    <row r="41" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L41"/>
+    </row>
+    <row r="42" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L42"/>
+    </row>
+    <row r="43" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L43"/>
+    </row>
+    <row r="44" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L44"/>
+    </row>
+    <row r="45" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L45"/>
+    </row>
+    <row r="46" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L46"/>
+    </row>
+    <row r="47" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L47"/>
+    </row>
+    <row r="48" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L48"/>
+    </row>
+    <row r="49" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L49"/>
+    </row>
+    <row r="50" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L50"/>
+    </row>
+    <row r="51" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L51"/>
+    </row>
+    <row r="52" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L52"/>
+    </row>
+    <row r="53" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L53"/>
+    </row>
+    <row r="54" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L54"/>
+    </row>
+    <row r="55" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L55"/>
+    </row>
+    <row r="56" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L56"/>
+    </row>
+    <row r="57" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L57"/>
+    </row>
+    <row r="58" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L58"/>
+    </row>
+    <row r="59" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L59"/>
+    </row>
+    <row r="60" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L60"/>
+    </row>
+    <row r="61" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L61"/>
+    </row>
+    <row r="62" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L62"/>
+    </row>
+    <row r="63" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L63"/>
+    </row>
+    <row r="64" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L64"/>
+    </row>
+    <row r="65" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L65"/>
+    </row>
+    <row r="66" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L66"/>
+    </row>
+    <row r="67" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L67"/>
+    </row>
+    <row r="68" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L68"/>
+    </row>
+    <row r="69" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L69"/>
+    </row>
+    <row r="70" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L70"/>
+    </row>
+    <row r="71" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L71"/>
+    </row>
+    <row r="72" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L72"/>
+    </row>
+    <row r="73" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L73"/>
+    </row>
+    <row r="74" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L74"/>
+    </row>
+    <row r="75" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L75"/>
+    </row>
+    <row r="76" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L76"/>
+    </row>
+    <row r="77" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L77"/>
+    </row>
+    <row r="78" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L78"/>
+    </row>
+    <row r="79" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L79"/>
+    </row>
+    <row r="80" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L80"/>
+    </row>
+    <row r="81" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L81"/>
+    </row>
+    <row r="82" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L82"/>
+    </row>
+    <row r="83" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L83"/>
+    </row>
+    <row r="84" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L84"/>
+    </row>
+    <row r="85" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L85"/>
+    </row>
+    <row r="86" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L86"/>
+    </row>
+    <row r="87" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L87"/>
+    </row>
+    <row r="88" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L88"/>
+    </row>
+    <row r="89" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L89"/>
+    </row>
+    <row r="90" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L90"/>
+    </row>
+    <row r="91" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L91"/>
+    </row>
+    <row r="92" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L92"/>
+    </row>
+    <row r="93" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L93"/>
+    </row>
+    <row r="94" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L94"/>
+    </row>
+    <row r="95" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L95"/>
+    </row>
+    <row r="96" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L96"/>
+    </row>
+    <row r="97" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L97"/>
+    </row>
+    <row r="98" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L98"/>
+    </row>
+    <row r="99" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L99"/>
+    </row>
+    <row r="100" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L100"/>
+    </row>
+    <row r="101" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L101"/>
+    </row>
+    <row r="102" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L102"/>
+    </row>
+    <row r="103" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L103"/>
+    </row>
+    <row r="104" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L104"/>
+    </row>
+    <row r="105" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L105"/>
+    </row>
+    <row r="106" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L106"/>
+    </row>
+    <row r="107" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L107"/>
+    </row>
+    <row r="108" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L108"/>
+    </row>
+    <row r="109" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L109"/>
+    </row>
+    <row r="110" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L110"/>
+    </row>
+    <row r="111" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L111"/>
+    </row>
+    <row r="112" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L112"/>
+    </row>
+    <row r="113" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L113"/>
+    </row>
+    <row r="114" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L114"/>
+    </row>
+    <row r="115" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L115"/>
+    </row>
+    <row r="116" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L116"/>
+    </row>
+    <row r="117" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L117"/>
+    </row>
+    <row r="118" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L118"/>
+    </row>
+    <row r="119" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L119"/>
+    </row>
+    <row r="120" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L120"/>
+    </row>
+    <row r="121" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L121"/>
+    </row>
+    <row r="122" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L122"/>
+    </row>
+    <row r="123" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L123"/>
+    </row>
+    <row r="124" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L124"/>
+    </row>
+    <row r="125" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L125"/>
+    </row>
+    <row r="126" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L126"/>
+    </row>
+    <row r="127" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L127"/>
+    </row>
+    <row r="128" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L128"/>
+    </row>
+    <row r="129" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L129"/>
+    </row>
+    <row r="130" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L130"/>
+    </row>
+    <row r="131" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L131"/>
+    </row>
+    <row r="132" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L132"/>
+    </row>
+    <row r="133" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L133"/>
+    </row>
+    <row r="134" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L134"/>
+    </row>
+    <row r="135" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L135"/>
+    </row>
+    <row r="136" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L136"/>
+    </row>
+    <row r="137" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L137"/>
+    </row>
+    <row r="138" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L138"/>
+    </row>
+    <row r="139" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L139"/>
+    </row>
+    <row r="140" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L140"/>
+    </row>
+    <row r="141" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L141"/>
+    </row>
+    <row r="142" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L142"/>
+    </row>
+    <row r="143" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L143"/>
+    </row>
+    <row r="144" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L144"/>
+    </row>
+    <row r="145" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L145"/>
+    </row>
+    <row r="146" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L146"/>
+    </row>
+    <row r="147" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L147"/>
+    </row>
+    <row r="148" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L148"/>
+    </row>
+    <row r="149" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L149"/>
+    </row>
+    <row r="150" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L150"/>
+    </row>
+    <row r="151" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L151"/>
+    </row>
+    <row r="152" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L152"/>
+    </row>
+    <row r="153" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L153"/>
+    </row>
+    <row r="154" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L154"/>
+    </row>
+    <row r="155" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L155"/>
+    </row>
+    <row r="156" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L156"/>
+    </row>
+    <row r="157" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L157"/>
+    </row>
+    <row r="158" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L158"/>
+    </row>
+    <row r="159" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L159"/>
+    </row>
+    <row r="160" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L160"/>
+    </row>
+    <row r="161" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L161"/>
+    </row>
+    <row r="162" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L162"/>
+    </row>
+    <row r="163" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L163"/>
+    </row>
+    <row r="164" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L164"/>
+    </row>
+    <row r="165" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L165"/>
+    </row>
+    <row r="166" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L166"/>
+    </row>
+    <row r="167" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L167"/>
+    </row>
+    <row r="168" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L168"/>
+    </row>
+    <row r="169" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L169"/>
+    </row>
+    <row r="170" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L170"/>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:V1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,21 +1198,28 @@
     <col min="2" max="2" width="18.7109375" customWidth="1"/>
     <col min="3" max="3" width="30.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="56.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="104" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="60.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="255.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" customWidth="1"/>
+    <col min="10" max="10" width="20.85546875" customWidth="1"/>
+    <col min="11" max="11" width="17.85546875" customWidth="1"/>
+    <col min="12" max="12" width="25" customWidth="1"/>
+    <col min="13" max="13" width="16.7109375" customWidth="1"/>
+    <col min="14" max="14" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="31.140625" customWidth="1"/>
+    <col min="17" max="17" width="38.42578125" customWidth="1"/>
+    <col min="18" max="18" width="52.85546875" customWidth="1"/>
+    <col min="19" max="19" width="15.28515625" customWidth="1"/>
+    <col min="20" max="20" width="14.28515625" customWidth="1"/>
+    <col min="21" max="21" width="17.85546875" customWidth="1"/>
+    <col min="22" max="22" width="33.85546875" customWidth="1"/>
+    <col min="23" max="23" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -648,43 +1233,62 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>17</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>18</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>13</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" t="s">
+        <v>19</v>
+      </c>
+      <c r="S1" t="s">
+        <v>29</v>
+      </c>
+      <c r="T1" t="s">
+        <v>30</v>
+      </c>
+      <c r="U1" t="s">
+        <v>31</v>
+      </c>
+      <c r="V1" t="s">
         <v>16</v>
       </c>
-      <c r="O1" t="s">
-        <v>19</v>
-      </c>
-      <c r="P1" t="s">
-        <v>14</v>
-      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -694,10 +1298,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -706,16 +1310,19 @@
     <col min="2" max="2" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="39.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="47.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="66.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="143.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.42578125" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" customWidth="1"/>
+    <col min="11" max="11" width="18.28515625" customWidth="1"/>
+    <col min="12" max="12" width="21.28515625" customWidth="1"/>
+    <col min="13" max="13" width="16.42578125" customWidth="1"/>
+    <col min="14" max="14" width="42.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -729,25 +1336,34 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" t="s">
         <v>20</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>21</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>22</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>23</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>24</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>25</v>
       </c>
-      <c r="K1" t="s">
-        <v>14</v>
+      <c r="N1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>